<commit_message>
some font size changes
</commit_message>
<xml_diff>
--- a/resources/OrderBackup.xlsx
+++ b/resources/OrderBackup.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="130">
   <si>
     <t>Type</t>
   </si>
@@ -53,58 +53,64 @@
     <t>Product Name</t>
   </si>
   <si>
-    <t/>
+    <t>Hudson Greens and Goods</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24 bu/cs</t>
+  </si>
+  <si>
+    <t>12/20/2022</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>RDF 1</t>
   </si>
   <si>
     <t>Red Mustard Greens,  24 bu/cs</t>
   </si>
   <si>
-    <t>12/20/2022</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 24 bu/cs</t>
-  </si>
-  <si>
-    <t>Hudson Greens and Goods</t>
-  </si>
-  <si>
-    <t>50.0</t>
+    <t>12246</t>
+  </si>
+  <si>
+    <t>818181022823</t>
   </si>
   <si>
     <t>RM24</t>
   </si>
   <si>
-    <t>Invoice</t>
+    <t>Caitlin</t>
   </si>
   <si>
     <t>Red Mustard Greens</t>
   </si>
   <si>
-    <t>12246</t>
-  </si>
-  <si>
-    <t>818181022823</t>
-  </si>
-  <si>
     <t>Red Russian Kale,  24 bu/cs</t>
   </si>
   <si>
+    <t>818181022854</t>
+  </si>
+  <si>
     <t>RRK24</t>
   </si>
   <si>
     <t>Red Russian Kale</t>
   </si>
   <si>
-    <t>818181022854</t>
+    <t>2.0</t>
   </si>
   <si>
     <t>Dino Kale,  24 bu/cs</t>
   </si>
   <si>
-    <t>2.0</t>
+    <t>818181022519</t>
   </si>
   <si>
     <t>DK24</t>
@@ -113,16 +119,16 @@
     <t>Dino Kale</t>
   </si>
   <si>
-    <t>818181022519</t>
+    <t>18.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 lbs/cs</t>
   </si>
   <si>
     <t>Savoy Spinach,  4 lbs/cs</t>
   </si>
   <si>
-    <t xml:space="preserve"> 4 lbs/cs</t>
-  </si>
-  <si>
-    <t>18.0</t>
+    <t>818181022885</t>
   </si>
   <si>
     <t>SP4</t>
@@ -131,19 +137,19 @@
     <t>Savoy Spinach</t>
   </si>
   <si>
-    <t>818181022885</t>
+    <t>87.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Size B/C, 25 lbs/cs</t>
+  </si>
+  <si>
+    <t>1.0</t>
   </si>
   <si>
     <t>Purple Majesty Potatoes,  Size B/C, 25 lbs/cs</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Size B/C, 25 lbs/cs</t>
-  </si>
-  <si>
-    <t>87.5</t>
+    <t>818181025107</t>
   </si>
   <si>
     <t>PMC25</t>
@@ -152,16 +158,16 @@
     <t>Purple Majesty Potatoes</t>
   </si>
   <si>
-    <t>818181025107</t>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3 lbs/cs</t>
   </si>
   <si>
     <t>Mixed Baby Kale,  3 lbs/cs</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3 lbs/cs</t>
-  </si>
-  <si>
-    <t>16.0</t>
+    <t>818181022687</t>
   </si>
   <si>
     <t>MXBK3</t>
@@ -170,40 +176,43 @@
     <t>Mixed Baby Kale</t>
   </si>
   <si>
-    <t>818181022687</t>
+    <t>Produce Express</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 lbs/cs,</t>
+  </si>
+  <si>
+    <t>10.0</t>
   </si>
   <si>
     <t>Bloomsdale Spinach,  4 lbs/cs,</t>
   </si>
   <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4 lbs/cs,</t>
-  </si>
-  <si>
-    <t>Produce Express</t>
+    <t>12245</t>
+  </si>
+  <si>
+    <t>818181022250</t>
   </si>
   <si>
     <t>BLSP4</t>
   </si>
   <si>
+    <t>RF-122022</t>
+  </si>
+  <si>
     <t>Bloomsdale Spinach</t>
   </si>
   <si>
-    <t>12245</t>
-  </si>
-  <si>
-    <t>818181022250</t>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
   </si>
   <si>
     <t>Braising Mix,  3 lbs/cs</t>
   </si>
   <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>14.0</t>
+    <t>818181022397</t>
   </si>
   <si>
     <t>BRMX3</t>
@@ -212,16 +221,16 @@
     <t>Braising Mix</t>
   </si>
   <si>
-    <t>818181022397</t>
+    <t>28.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20 lb/cs,</t>
   </si>
   <si>
     <t>King Richard Leeks,  20 lb/cs,</t>
   </si>
   <si>
-    <t xml:space="preserve"> 20 lb/cs,</t>
-  </si>
-  <si>
-    <t>28.0</t>
+    <t>818181023462</t>
   </si>
   <si>
     <t>KRL20</t>
@@ -230,13 +239,13 @@
     <t>King Richard Leeks</t>
   </si>
   <si>
-    <t>818181023462</t>
+    <t>32.0</t>
   </si>
   <si>
     <t>Tokyo Turnips,  24 bu/cs</t>
   </si>
   <si>
-    <t>32.0</t>
+    <t>818181027583</t>
   </si>
   <si>
     <t>TT24</t>
@@ -245,16 +254,16 @@
     <t>Tokyo Turnips</t>
   </si>
   <si>
-    <t>818181027583</t>
+    <t>70.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Size B, 25 lbs/cs</t>
   </si>
   <si>
     <t>German Butterball Potatoes,  Size B, 25 lbs/cs</t>
   </si>
   <si>
-    <t xml:space="preserve"> Size B, 25 lbs/cs</t>
-  </si>
-  <si>
-    <t>70.0</t>
+    <t>818181024889</t>
   </si>
   <si>
     <t>GBBB25</t>
@@ -263,79 +272,82 @@
     <t>German Butterball Potatoes</t>
   </si>
   <si>
-    <t>818181024889</t>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12 bu/cs</t>
+  </si>
+  <si>
+    <t>30.0</t>
   </si>
   <si>
     <t>Dino Kale,  12 bu/cs</t>
   </si>
   <si>
-    <t>30.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12 bu/cs</t>
-  </si>
-  <si>
-    <t>15.0</t>
+    <t>818181022496</t>
   </si>
   <si>
     <t>DK12</t>
   </si>
   <si>
-    <t>818181022496</t>
+    <t>SNFC</t>
+  </si>
+  <si>
+    <t>13.0</t>
   </si>
   <si>
     <t>Thyme,  12 bu/cs</t>
   </si>
   <si>
-    <t>SNFC</t>
-  </si>
-  <si>
-    <t>13.0</t>
+    <t>12244</t>
+  </si>
+  <si>
+    <t>818181023127</t>
   </si>
   <si>
     <t>THYME</t>
   </si>
   <si>
+    <t>Kate</t>
+  </si>
+  <si>
     <t>Thyme</t>
   </si>
   <si>
-    <t>12244</t>
-  </si>
-  <si>
-    <t>818181023127</t>
-  </si>
-  <si>
     <t>Green Mustard Greens,  24 bu/cs</t>
   </si>
   <si>
+    <t>818181022595</t>
+  </si>
+  <si>
     <t>GM24</t>
   </si>
   <si>
     <t>Green Mustard Greens</t>
   </si>
   <si>
-    <t>818181022595</t>
-  </si>
-  <si>
     <t>Spinach,  24 bu/cs</t>
   </si>
   <si>
+    <t>818181022861</t>
+  </si>
+  <si>
     <t>SP24</t>
   </si>
   <si>
     <t>Spinach</t>
   </si>
   <si>
-    <t>818181022861</t>
+    <t>42.0</t>
+  </si>
+  <si>
+    <t>8.0</t>
   </si>
   <si>
     <t>Curly Kale,  24 bu/cs</t>
   </si>
   <si>
-    <t>8.0</t>
-  </si>
-  <si>
-    <t>42.0</t>
+    <t>818181022458</t>
   </si>
   <si>
     <t>CK24</t>
@@ -344,28 +356,28 @@
     <t>Curly Kale</t>
   </si>
   <si>
-    <t>818181022458</t>
-  </si>
-  <si>
     <t>9.0</t>
   </si>
   <si>
     <t>Collard Greens,  24 bu/cs</t>
   </si>
   <si>
+    <t>818181022489</t>
+  </si>
+  <si>
     <t>COL24</t>
   </si>
   <si>
     <t>Collard Greens</t>
   </si>
   <si>
-    <t>818181022489</t>
+    <t xml:space="preserve"> 25 lbs/bag</t>
   </si>
   <si>
     <t>Purple Top Turnips,  25 lbs/bag</t>
   </si>
   <si>
-    <t xml:space="preserve"> 25 lbs/bag</t>
+    <t>818181027514</t>
   </si>
   <si>
     <t>PTT25</t>
@@ -374,25 +386,22 @@
     <t>Purple Top Turnips</t>
   </si>
   <si>
-    <t>818181027514</t>
+    <t>45.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20 lbs/cs</t>
   </si>
   <si>
     <t>Mei Qing Choi,  20 lbs/cs</t>
   </si>
   <si>
-    <t xml:space="preserve"> 20 lbs/cs</t>
-  </si>
-  <si>
-    <t>45.0</t>
+    <t>818181022656</t>
   </si>
   <si>
     <t>MQC20</t>
   </si>
   <si>
     <t>Mei Qing Choi</t>
-  </si>
-  <si>
-    <t>818181022656</t>
   </si>
 </sst>
 </file>
@@ -486,904 +495,904 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
       </c>
       <c r="J4" t="s">
         <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
         <v>39</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>37</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
       </c>
       <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
         <v>36</v>
       </c>
-      <c r="L5" t="s">
-        <v>35</v>
-      </c>
       <c r="M5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
         <v>46</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>44</v>
       </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
       <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
         <v>41</v>
-      </c>
-      <c r="K6" t="s">
-        <v>43</v>
       </c>
       <c r="L6" t="s">
         <v>42</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
         <v>52</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>50</v>
-      </c>
-      <c r="I7" t="s">
-        <v>47</v>
       </c>
       <c r="J7" t="s">
         <v>30</v>
       </c>
       <c r="K7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" t="s">
         <v>49</v>
       </c>
-      <c r="L7" t="s">
-        <v>48</v>
-      </c>
       <c r="M7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
         <v>56</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" t="s">
-        <v>54</v>
-      </c>
       <c r="K8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L8" t="s">
         <v>55</v>
       </c>
       <c r="M8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
         <v>66</v>
       </c>
       <c r="H9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" t="s">
         <v>64</v>
-      </c>
-      <c r="I9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" t="s">
-        <v>62</v>
       </c>
       <c r="K9" t="s">
         <v>63</v>
       </c>
       <c r="L9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
         <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="J10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K10" t="s">
         <v>69</v>
       </c>
       <c r="L10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="M10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G11" t="s">
         <v>77</v>
       </c>
       <c r="H11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" t="s">
         <v>75</v>
       </c>
-      <c r="I11" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" t="s">
-        <v>74</v>
-      </c>
       <c r="L11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
         <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K12" t="s">
         <v>80</v>
       </c>
       <c r="L12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" t="s">
         <v>89</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>88</v>
       </c>
-      <c r="I13" t="s">
-        <v>84</v>
-      </c>
-      <c r="J13" t="s">
-        <v>85</v>
-      </c>
       <c r="K13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" t="s">
         <v>87</v>
       </c>
-      <c r="L13" t="s">
-        <v>86</v>
-      </c>
       <c r="M13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G14" t="s">
         <v>96</v>
       </c>
       <c r="H14" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="I14" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="J14" t="s">
         <v>30</v>
       </c>
       <c r="K14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M14" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
         <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" t="s">
         <v>100</v>
       </c>
-      <c r="H15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" t="s">
-        <v>97</v>
-      </c>
       <c r="J15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M15" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
         <v>95</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s">
         <v>20</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" t="s">
         <v>14</v>
       </c>
-      <c r="J16" t="s">
-        <v>41</v>
-      </c>
-      <c r="K16" t="s">
-        <v>19</v>
-      </c>
       <c r="L16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M16" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
         <v>95</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" t="s">
         <v>104</v>
       </c>
-      <c r="H17" t="s">
-        <v>102</v>
-      </c>
-      <c r="I17" t="s">
-        <v>101</v>
-      </c>
       <c r="J17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>95</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G18" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" t="s">
         <v>110</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
+        <v>109</v>
+      </c>
+      <c r="K18" t="s">
         <v>108</v>
       </c>
-      <c r="I18" t="s">
-        <v>105</v>
-      </c>
-      <c r="J18" t="s">
-        <v>106</v>
-      </c>
-      <c r="K18" t="s">
-        <v>107</v>
-      </c>
       <c r="L18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M18" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
         <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" t="s">
         <v>33</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>31</v>
       </c>
-      <c r="I19" t="s">
-        <v>29</v>
-      </c>
       <c r="J19" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="K19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
         <v>95</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" t="s">
         <v>115</v>
       </c>
-      <c r="H20" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" t="s">
-        <v>112</v>
-      </c>
       <c r="J20" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="K20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
         <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G21" t="s">
         <v>66</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I21" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="J21" t="s">
         <v>30</v>
       </c>
       <c r="K21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L21" t="s">
         <v>49</v>
       </c>
-      <c r="L21" t="s">
-        <v>48</v>
-      </c>
       <c r="M21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
         <v>95</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" t="s">
         <v>120</v>
       </c>
-      <c r="H22" t="s">
-        <v>118</v>
-      </c>
-      <c r="I22" t="s">
-        <v>116</v>
-      </c>
       <c r="J22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K22" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L22" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M22" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
         <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G23" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" t="s">
         <v>126</v>
-      </c>
-      <c r="H23" t="s">
-        <v>124</v>
-      </c>
-      <c r="I23" t="s">
-        <v>121</v>
       </c>
       <c r="J23" t="s">
         <v>30</v>
       </c>
       <c r="K23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L23" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="M23" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>